<commit_message>
updated TestContext for Background
</commit_message>
<xml_diff>
--- a/Team04_RestfulRebels/src/test/resources/TestData/Team04_RestfulRebels.xlsx
+++ b/Team04_RestfulRebels/src/test/resources/TestData/Team04_RestfulRebels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="88">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -181,46 +181,112 @@
     <t>classRecordingPath</t>
   </si>
   <si>
+    <t>2025-11-21T15:11:08.750+00:00</t>
+  </si>
+  <si>
+    <t>Tamil</t>
+  </si>
+  <si>
+    <t>Starting ch 1</t>
+  </si>
+  <si>
+    <t>Basic to Advance</t>
+  </si>
+  <si>
+    <t>Test notes</t>
+  </si>
+  <si>
+    <t>C:/Recordings</t>
+  </si>
+  <si>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>post</t>
+  </si>
+  <si>
+    <t>PythonAyanae</t>
+  </si>
+  <si>
+    <t>TC_02_class</t>
+  </si>
+  <si>
+    <t>Tamilab</t>
+  </si>
+  <si>
+    <t>TC_03_class</t>
+  </si>
+  <si>
+    <t>Starting ch 2</t>
+  </si>
+  <si>
+    <t>TC_04_class</t>
+  </si>
+  <si>
+    <t>valid data</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>Additional</t>
+  </si>
+  <si>
+    <t>invalid data</t>
+  </si>
+  <si>
+    <t>ClassUsecases</t>
+  </si>
+  <si>
+    <t xml:space="preserve">valid </t>
+  </si>
+  <si>
+    <t>U1234</t>
+  </si>
+  <si>
+    <t>existing class topic</t>
+  </si>
+  <si>
+    <t>Tamilac</t>
+  </si>
+  <si>
+    <t>TC_05_class</t>
+  </si>
+  <si>
+    <t>TC_06_class</t>
+  </si>
+  <si>
+    <t>batchIdUseCase</t>
+  </si>
+  <si>
+    <t>classStaffIdUseCase</t>
+  </si>
+  <si>
+    <t>notvalid</t>
+  </si>
+  <si>
     <t>classScheduledDates_1</t>
   </si>
   <si>
     <t>classScheduledDates_2</t>
   </si>
   <si>
-    <t>2025-11-21T15:11:08.750+00:00</t>
-  </si>
-  <si>
-    <t>Tamil</t>
-  </si>
-  <si>
-    <t>Starting ch 1</t>
-  </si>
-  <si>
-    <t>Basic to Advance</t>
-  </si>
-  <si>
-    <t>Test notes</t>
-  </si>
-  <si>
-    <t>C:/Recordings</t>
-  </si>
-  <si>
     <t>2025-11-22T15:11:08.750+00:00</t>
   </si>
   <si>
-    <t>2025-11-21T15:11:08.750+00:00,2025-11-22T15:11:08.750+00:00</t>
-  </si>
-  <si>
-    <t>Method</t>
-  </si>
-  <si>
-    <t>post</t>
+    <t>2025-11-23T15:11:08.750+00:00</t>
+  </si>
+  <si>
+    <t>2025-11-24T15:11:08.750+00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid Endpoint </t>
   </si>
   <si>
     <t>Class_GET_AllClassList</t>
   </si>
   <si>
-    <t>PythonAyanae</t>
+    <t>Endpointusecase</t>
   </si>
 </sst>
 </file>
@@ -713,7 +779,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -727,6 +793,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1107,7 +1176,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1275,8 +1344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1336,7 +1405,7 @@
         <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
         <v>39</v>
@@ -1401,145 +1470,423 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A9:T11"/>
+  <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="14.5" customWidth="1"/>
-    <col min="14" max="14" width="17.09765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.69921875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="14.5" customWidth="1"/>
+    <col min="17" max="17" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="27.796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:20">
-      <c r="A9" t="s">
+    <row r="1" spans="1:23">
+      <c r="A1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>51</v>
+      </c>
+      <c r="R1" t="s">
+        <v>80</v>
+      </c>
+      <c r="S1" t="s">
+        <v>81</v>
+      </c>
+      <c r="T1" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2">
+        <v>2</v>
+      </c>
+      <c r="I2" t="s">
+        <v>52</v>
+      </c>
+      <c r="J2" t="s">
+        <v>53</v>
+      </c>
+      <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S2" t="s">
+        <v>82</v>
+      </c>
+      <c r="T2" t="s">
+        <v>86</v>
+      </c>
+      <c r="U2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23">
+      <c r="A3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2">
+        <v>2</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J3" t="s">
         <v>62</v>
       </c>
-      <c r="C9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" t="s">
-        <v>43</v>
-      </c>
-      <c r="G9" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" t="s">
-        <v>45</v>
-      </c>
-      <c r="I9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" t="s">
-        <v>48</v>
-      </c>
-      <c r="L9" t="s">
-        <v>49</v>
-      </c>
-      <c r="M9" t="s">
-        <v>50</v>
-      </c>
-      <c r="N9" t="s">
-        <v>51</v>
-      </c>
-      <c r="O9" t="s">
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R3" t="s">
+        <v>83</v>
+      </c>
+      <c r="S3" t="s">
+        <v>84</v>
+      </c>
+      <c r="U3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23">
+      <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="L4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23">
+      <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>79</v>
+      </c>
+      <c r="G5">
+        <v>12345</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2</v>
+      </c>
+      <c r="I5" t="s">
         <v>52</v>
       </c>
-      <c r="P9" t="s">
+      <c r="J5" t="s">
+        <v>74</v>
+      </c>
+      <c r="K5" t="s">
+        <v>39</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" t="s">
+        <v>54</v>
+      </c>
+      <c r="O5" t="s">
+        <v>55</v>
+      </c>
+      <c r="P5" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>57</v>
+      </c>
+      <c r="R5" t="s">
+        <v>52</v>
+      </c>
+      <c r="S5" t="s">
+        <v>82</v>
+      </c>
+      <c r="U5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="27.6">
+      <c r="A6" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+      <c r="I6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" t="s">
         <v>53</v>
       </c>
-      <c r="Q9" t="s">
-        <v>1</v>
-      </c>
-      <c r="R9" t="s">
-        <v>20</v>
-      </c>
-      <c r="S9" t="s">
-        <v>21</v>
-      </c>
-      <c r="T9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20">
-      <c r="A10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="K6" t="s">
+        <v>39</v>
+      </c>
+      <c r="L6" t="s">
         <v>16</v>
       </c>
-      <c r="D10" t="s">
+      <c r="N6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" t="s">
+        <v>55</v>
+      </c>
+      <c r="P6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>57</v>
+      </c>
+      <c r="R6" t="s">
+        <v>52</v>
+      </c>
+      <c r="S6" t="s">
+        <v>82</v>
+      </c>
+      <c r="U6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="F10">
+      <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2">
         <v>2</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I7" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" t="s">
+        <v>39</v>
+      </c>
+      <c r="L7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N7" t="s">
         <v>54</v>
       </c>
-      <c r="H10" t="s">
+      <c r="O7" t="s">
         <v>55</v>
       </c>
-      <c r="I10" t="s">
-        <v>39</v>
-      </c>
-      <c r="K10" t="s">
+      <c r="P7" t="s">
         <v>56</v>
       </c>
-      <c r="L10" t="s">
+      <c r="Q7" t="s">
         <v>57</v>
       </c>
-      <c r="M10" t="s">
-        <v>58</v>
-      </c>
-      <c r="N10" t="s">
-        <v>59</v>
-      </c>
-      <c r="O10" t="s">
-        <v>61</v>
-      </c>
-      <c r="P10" t="s">
-        <v>60</v>
-      </c>
-      <c r="R10">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20">
-      <c r="B11" t="s">
-        <v>64</v>
+      <c r="R7" t="s">
+        <v>52</v>
+      </c>
+      <c r="S7" t="s">
+        <v>82</v>
+      </c>
+      <c r="T7" t="s">
+        <v>86</v>
+      </c>
+      <c r="U7">
+        <v>404</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated cleanup, schema validation
</commit_message>
<xml_diff>
--- a/Team04_RestfulRebels/src/test/resources/TestData/Team04_RestfulRebels.xlsx
+++ b/Team04_RestfulRebels/src/test/resources/TestData/Team04_RestfulRebels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4"/>
+    <workbookView minimized="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="152">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -100,9 +100,6 @@
     <t>expectedErrormessage</t>
   </si>
   <si>
-    <t>Note: Only defined users succeed registration</t>
-  </si>
-  <si>
     <t>TC_04_login</t>
   </si>
   <si>
@@ -148,9 +145,6 @@
     <t>Apiphase@2</t>
   </si>
   <si>
-    <t>TC_01_class</t>
-  </si>
-  <si>
     <t>batchId</t>
   </si>
   <si>
@@ -181,9 +175,6 @@
     <t>2025-11-21T15:11:08.750+00:00</t>
   </si>
   <si>
-    <t>Tamil</t>
-  </si>
-  <si>
     <t>Starting ch 1</t>
   </si>
   <si>
@@ -205,21 +196,9 @@
     <t>PythonAyanae</t>
   </si>
   <si>
-    <t>TC_02_class</t>
-  </si>
-  <si>
-    <t>Tamilab</t>
-  </si>
-  <si>
-    <t>TC_03_class</t>
-  </si>
-  <si>
     <t>Starting ch 2</t>
   </si>
   <si>
-    <t>TC_04_class</t>
-  </si>
-  <si>
     <t>Mandatory</t>
   </si>
   <si>
@@ -229,15 +208,6 @@
     <t xml:space="preserve">valid </t>
   </si>
   <si>
-    <t>Tamilac</t>
-  </si>
-  <si>
-    <t>TC_05_class</t>
-  </si>
-  <si>
-    <t>TC_06_class</t>
-  </si>
-  <si>
     <t>elamathi</t>
   </si>
   <si>
@@ -268,81 +238,42 @@
     <t>abc</t>
   </si>
   <si>
-    <t>vaild</t>
-  </si>
-  <si>
-    <t>2025-11-2&amp;&amp;&amp;&amp;1T15:11:08.750+00:00</t>
-  </si>
-  <si>
     <t>Tamil16</t>
   </si>
   <si>
     <t>invalidEndpoint</t>
   </si>
   <si>
-    <t>TC_07_class</t>
-  </si>
-  <si>
     <t>empty</t>
   </si>
   <si>
-    <t>TC_08_class</t>
-  </si>
-  <si>
-    <t>Tamil08</t>
-  </si>
-  <si>
     <t>class_get_allclasslist</t>
   </si>
   <si>
-    <t>TC_09_class</t>
-  </si>
-  <si>
-    <t>TC_10_class</t>
-  </si>
-  <si>
     <t>wrong method</t>
   </si>
   <si>
     <t>ClassId</t>
   </si>
   <si>
-    <t>TC_11_class</t>
-  </si>
-  <si>
     <t>byBatchId</t>
   </si>
   <si>
     <t>class_get_classrecordings_bybatchid</t>
   </si>
   <si>
-    <t>TC_12_class</t>
-  </si>
-  <si>
     <t>byinvalidBatchId</t>
   </si>
   <si>
     <t>efghi</t>
   </si>
   <si>
-    <t>TC_13_class</t>
-  </si>
-  <si>
-    <t>TC_14_class</t>
-  </si>
-  <si>
     <t>byTopic</t>
   </si>
   <si>
-    <t>byinvalidTopic</t>
-  </si>
-  <si>
     <t>Topic</t>
   </si>
   <si>
-    <t>TC_15_class</t>
-  </si>
-  <si>
     <t>class_get_byclasstopic</t>
   </si>
   <si>
@@ -352,17 +283,214 @@
     <t>45Tr$</t>
   </si>
   <si>
-    <t>TC_16_class</t>
-  </si>
-  <si>
-    <t>TC_17_class</t>
+    <t>saveprogram</t>
+  </si>
+  <si>
+    <t>Tamil10</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 201 Created</t>
+  </si>
+  <si>
+    <t>Tamilab3</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 404 Not Found</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 405 Method Not Allowed</t>
+  </si>
+  <si>
+    <t>/batchRecordingstpyhon</t>
+  </si>
+  <si>
+    <t>Active User with given email Id Not Found</t>
+  </si>
+  <si>
+    <t>password must contain atleast 8 to max 32 characters, a capital letter, a small letter, a special character, a number and no space</t>
+  </si>
+  <si>
+    <t>empty username</t>
+  </si>
+  <si>
+    <t>expectedErrorMessage</t>
+  </si>
+  <si>
+    <t>TC_06_login</t>
+  </si>
+  <si>
+    <t>empty password</t>
+  </si>
+  <si>
+    <t>EmailId is mandatory</t>
+  </si>
+  <si>
+    <t>HTTP/1.1 401 Unauthorized</t>
+  </si>
+  <si>
+    <t>Password is mandatory</t>
+  </si>
+  <si>
+    <t>userComments</t>
+  </si>
+  <si>
+    <t>userEduPg</t>
+  </si>
+  <si>
+    <t>userEduUg</t>
+  </si>
+  <si>
+    <t>userFirstName</t>
+  </si>
+  <si>
+    <t>userLastName</t>
+  </si>
+  <si>
+    <t>userLinkedinUrl</t>
+  </si>
+  <si>
+    <t>userLocation</t>
+  </si>
+  <si>
+    <t>userMiddleName</t>
+  </si>
+  <si>
+    <t>userPhoneNumber</t>
+  </si>
+  <si>
+    <t>userTimeZone</t>
+  </si>
+  <si>
+    <t>userVisaStatus</t>
+  </si>
+  <si>
+    <t>loginStatus</t>
+  </si>
+  <si>
+    <t>userLoginEmail</t>
+  </si>
+  <si>
+    <t>roleId</t>
+  </si>
+  <si>
+    <t>userRoleStatus</t>
+  </si>
+  <si>
+    <t>NN Users of SDET</t>
+  </si>
+  <si>
+    <t>B.E</t>
+  </si>
+  <si>
+    <t>M.S</t>
+  </si>
+  <si>
+    <t>TeamFour</t>
+  </si>
+  <si>
+    <t>RestAssured</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/</t>
+  </si>
+  <si>
+    <t>NYC</t>
+  </si>
+  <si>
+    <t>Andy</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>R03</t>
+  </si>
+  <si>
+    <t>nnteam5@gmail.com</t>
+  </si>
+  <si>
+    <t>+91 1016213107</t>
+  </si>
+  <si>
+    <t>TC_01_class_post</t>
+  </si>
+  <si>
+    <t>TC_02_class_post</t>
+  </si>
+  <si>
+    <t>TC_03_class_post</t>
+  </si>
+  <si>
+    <t>TC_04_class_post</t>
+  </si>
+  <si>
+    <t>TC_05_class_post</t>
+  </si>
+  <si>
+    <t>TC_06_class_post</t>
+  </si>
+  <si>
+    <t>TC_07_class_post</t>
+  </si>
+  <si>
+    <t>TC_01_class_get</t>
+  </si>
+  <si>
+    <t>TC_02_class_get</t>
+  </si>
+  <si>
+    <t>TC_03_class_get</t>
+  </si>
+  <si>
+    <t>TC_04_class_get</t>
+  </si>
+  <si>
+    <t>TC_05_class_get</t>
+  </si>
+  <si>
+    <t>TC_06_class_get</t>
+  </si>
+  <si>
+    <t>TC_07_class_get</t>
+  </si>
+  <si>
+    <t>TC_09_class_get</t>
+  </si>
+  <si>
+    <t>TC_08_class_get</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+TC_10_class_get
+</t>
+  </si>
+  <si>
+    <t>TC_11_class_get</t>
+  </si>
+  <si>
+    <t>TC_01_class_del</t>
+  </si>
+  <si>
+    <t>valid classId</t>
+  </si>
+  <si>
+    <t>class_delete_byclassid</t>
+  </si>
+  <si>
+    <t>Tamil100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -505,6 +633,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF4EA72E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -688,18 +828,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -814,6 +954,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -860,7 +1015,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -876,9 +1031,40 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1255,10 +1441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1271,7 +1457,7 @@
     <col min="6" max="6" width="11.3984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.59765625" customWidth="1"/>
+    <col min="9" max="9" width="40.09765625" customWidth="1"/>
     <col min="12" max="12" width="14.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1301,7 +1487,7 @@
         <v>20</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -1315,7 +1501,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G2">
         <v>200</v>
@@ -1341,7 +1527,7 @@
         <v>7</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="G3" s="5">
         <v>400</v>
@@ -1350,38 +1536,41 @@
         <v>22</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="11" customFormat="1" ht="41.4">
+      <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" t="s">
-        <v>66</v>
-      </c>
-      <c r="G4">
+      <c r="E4" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="11">
         <v>400</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="11" t="s">
         <v>22</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -1389,31 +1578,64 @@
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="F5" t="s">
         <v>18</v>
       </c>
       <c r="G5">
         <v>401</v>
       </c>
-      <c r="H5">
-        <v>401</v>
+      <c r="H5" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="5">
+        <v>400</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>39</v>
+      <c r="E7" s="1"/>
+      <c r="G7" s="5">
+        <v>400</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1422,12 +1644,11 @@
     <hyperlink ref="E3" r:id="rId2"/>
     <hyperlink ref="D4" r:id="rId3"/>
     <hyperlink ref="E4" r:id="rId4" display="March@"/>
-    <hyperlink ref="D5" r:id="rId5"/>
-    <hyperlink ref="E5" r:id="rId6"/>
-    <hyperlink ref="E6" r:id="rId7"/>
-    <hyperlink ref="D6" r:id="rId8"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+    <hyperlink ref="D7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1435,16 +1656,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.69921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.296875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.69921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
@@ -1461,13 +1684,13 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
         <v>36</v>
-      </c>
-      <c r="F1" t="s">
-        <v>37</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
@@ -1484,22 +1707,22 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2">
         <v>201</v>
@@ -1507,27 +1730,48 @@
     </row>
     <row r="3" spans="1:10">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" t="s">
+        <v>85</v>
+      </c>
+      <c r="H3">
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1549,32 +1793,192 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.19921875" customWidth="1"/>
+    <col min="2" max="2" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.796875" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="6" customFormat="1" ht="14.4" thickBot="1">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="R1" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="S1" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="T1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+    </row>
+    <row r="2" spans="1:26" s="11" customFormat="1" ht="28.2" thickBot="1">
+      <c r="A2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>126</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="R2" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="S2" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="15"/>
+      <c r="U2" s="18">
+        <v>201</v>
+      </c>
+      <c r="V2" s="15"/>
+      <c r="W2" s="15"/>
+      <c r="X2" s="15"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" display="http://www.linkedin.com/"/>
+    <hyperlink ref="Q2" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="31.19921875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.8984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="27.796875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.09765625" bestFit="1" customWidth="1"/>
@@ -1587,8 +1991,9 @@
     <col min="17" max="17" width="55.5" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="9.69921875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="9.69921875" customWidth="1"/>
+    <col min="20" max="20" width="20.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.19921875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1600,55 +2005,55 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="F1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
         <v>41</v>
       </c>
-      <c r="G1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>42</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
         <v>43</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="K1" t="s">
-        <v>72</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="O1" t="s">
         <v>46</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>47</v>
       </c>
-      <c r="O1" t="s">
-        <v>48</v>
-      </c>
-      <c r="P1" t="s">
-        <v>49</v>
-      </c>
       <c r="Q1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R1" t="s">
         <v>75</v>
       </c>
-      <c r="R1" t="s">
-        <v>92</v>
-      </c>
       <c r="S1" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="T1" t="s">
         <v>1</v>
@@ -1665,13 +2070,13 @@
     </row>
     <row r="2" spans="1:23">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
         <v>15</v>
@@ -1683,45 +2088,48 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" t="s">
+        <v>151</v>
+      </c>
+      <c r="J2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" t="s">
+        <v>49</v>
+      </c>
+      <c r="N2" t="s">
         <v>50</v>
       </c>
-      <c r="I2" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+      <c r="P2" t="s">
         <v>52</v>
       </c>
-      <c r="N2" t="s">
-        <v>53</v>
-      </c>
-      <c r="O2" t="s">
-        <v>54</v>
-      </c>
-      <c r="P2" t="s">
-        <v>55</v>
-      </c>
       <c r="Q2" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="U2">
         <v>201</v>
       </c>
+      <c r="V2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="3" spans="1:23">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>15</v>
@@ -1733,33 +2141,36 @@
         <v>2</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K3" t="s">
         <v>15</v>
       </c>
       <c r="Q3" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="U3">
         <v>201</v>
       </c>
+      <c r="V3" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="4" spans="1:23">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>132</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -1771,83 +2182,86 @@
         <v>15</v>
       </c>
       <c r="M4" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="N4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="O4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="P4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="U4">
         <v>400</v>
       </c>
+      <c r="V4" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" t="s">
-        <v>63</v>
+      <c r="A5" s="8" t="s">
+        <v>133</v>
       </c>
       <c r="B5" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
         <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>80</v>
-      </c>
-      <c r="F5">
-        <v>12345</v>
+        <v>15</v>
       </c>
       <c r="G5">
         <v>2</v>
       </c>
       <c r="H5" t="s">
-        <v>81</v>
-      </c>
-      <c r="I5" t="s">
-        <v>67</v>
+        <v>48</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>89</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" t="s">
         <v>15</v>
       </c>
       <c r="M5" t="s">
+        <v>49</v>
+      </c>
+      <c r="N5" t="s">
+        <v>50</v>
+      </c>
+      <c r="O5" t="s">
+        <v>51</v>
+      </c>
+      <c r="P5" t="s">
         <v>52</v>
       </c>
-      <c r="N5" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" t="s">
-        <v>54</v>
-      </c>
-      <c r="P5" t="s">
-        <v>55</v>
-      </c>
       <c r="Q5" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="U5">
         <v>400</v>
       </c>
+      <c r="V5" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="6" spans="1:23">
       <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
         <v>68</v>
       </c>
-      <c r="B6" t="s">
-        <v>78</v>
-      </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -1859,45 +2273,48 @@
         <v>2</v>
       </c>
       <c r="H6" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N6" t="s">
         <v>50</v>
       </c>
-      <c r="I6" t="s">
+      <c r="O6" t="s">
         <v>51</v>
       </c>
-      <c r="J6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="P6" t="s">
         <v>52</v>
       </c>
-      <c r="N6" t="s">
-        <v>53</v>
-      </c>
-      <c r="O6" t="s">
-        <v>54</v>
-      </c>
-      <c r="P6" t="s">
-        <v>55</v>
-      </c>
       <c r="Q6" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="U6">
         <v>400</v>
       </c>
+      <c r="V6" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:23">
       <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>83</v>
+        <v>135</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>71</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -1909,48 +2326,51 @@
         <v>2</v>
       </c>
       <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" t="s">
+        <v>70</v>
+      </c>
+      <c r="J7" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" t="s">
+        <v>49</v>
+      </c>
+      <c r="N7" t="s">
         <v>50</v>
       </c>
-      <c r="I7" t="s">
-        <v>82</v>
-      </c>
-      <c r="J7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="O7" t="s">
+        <v>51</v>
+      </c>
+      <c r="P7" t="s">
         <v>52</v>
       </c>
-      <c r="N7" t="s">
-        <v>53</v>
-      </c>
-      <c r="O7" t="s">
-        <v>54</v>
-      </c>
-      <c r="P7" t="s">
-        <v>55</v>
-      </c>
       <c r="Q7" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="T7" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="U7">
         <v>404</v>
       </c>
+      <c r="V7" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="8" spans="1:23">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -1961,75 +2381,105 @@
       <c r="K8" t="s">
         <v>13</v>
       </c>
+      <c r="U8">
+        <v>400</v>
+      </c>
+      <c r="V8" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:23">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>137</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
+      </c>
+      <c r="U9">
+        <v>200</v>
+      </c>
+      <c r="V9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:23">
       <c r="A10" t="s">
-        <v>89</v>
+        <v>138</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
       <c r="T10" t="s">
-        <v>79</v>
+        <v>69</v>
+      </c>
+      <c r="U10">
+        <v>404</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:23">
       <c r="A11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B11" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="U11">
+        <v>405</v>
+      </c>
+      <c r="V11" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C11" t="s">
-        <v>88</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:23">
       <c r="A12" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>94</v>
+        <v>140</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C12" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
+      </c>
+      <c r="U12">
+        <v>200</v>
+      </c>
+      <c r="V12" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:23">
       <c r="A13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>97</v>
+        <v>141</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="C13" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -2037,92 +2487,169 @@
       <c r="F13">
         <v>12345</v>
       </c>
+      <c r="U13">
+        <v>404</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="14" spans="1:23">
       <c r="A14" t="s">
-        <v>99</v>
+        <v>142</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
       </c>
       <c r="T14" t="s">
-        <v>98</v>
+        <v>79</v>
+      </c>
+      <c r="U14">
+        <v>404</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:23">
       <c r="A15" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="U15">
+        <v>405</v>
+      </c>
+      <c r="V15" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C15" t="s">
-        <v>95</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:23">
       <c r="A16" t="s">
-        <v>104</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>101</v>
+        <v>145</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="C16" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="D16" t="s">
         <v>15</v>
       </c>
       <c r="S16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19">
+        <v>83</v>
+      </c>
+      <c r="U16">
+        <v>200</v>
+      </c>
+      <c r="V16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" t="s">
-        <v>108</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>101</v>
+        <v>144</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="C17" t="s">
-        <v>105</v>
+        <v>82</v>
       </c>
       <c r="D17" t="s">
         <v>15</v>
       </c>
       <c r="S17" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19">
-      <c r="A18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C18" t="s">
-        <v>105</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="S18" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19">
-      <c r="B23" t="s">
-        <v>102</v>
+        <v>84</v>
+      </c>
+      <c r="U17">
+        <v>404</v>
+      </c>
+      <c r="V17" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" s="11" customFormat="1" ht="41.4">
+      <c r="A18" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="C18" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="S18" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="U18" s="11">
+        <v>405</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>82</v>
+      </c>
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="T19" t="s">
+        <v>92</v>
+      </c>
+      <c r="U19">
+        <v>404</v>
+      </c>
+      <c r="V19" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C20" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="U20">
+        <v>200</v>
+      </c>
+      <c r="V20" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated unautscenatio invalid url and cleanup
</commit_message>
<xml_diff>
--- a/Team04_RestfulRebels/src/test/resources/TestData/Team04_RestfulRebels.xlsx
+++ b/Team04_RestfulRebels/src/test/resources/TestData/Team04_RestfulRebels.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,14 @@
     <sheet name="class" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="M">class!$H:$H</definedName>
+    <definedName name="M">class!$I:$I</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="243">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -229,9 +229,6 @@
     <t>2025-11-23T15:11:08.750+00:00,2025-11-24T15:11:08.750+00:00</t>
   </si>
   <si>
-    <t>Invalid Data</t>
-  </si>
-  <si>
     <t>Existing</t>
   </si>
   <si>
@@ -271,9 +268,6 @@
     <t>byTopic</t>
   </si>
   <si>
-    <t>Topic</t>
-  </si>
-  <si>
     <t>class_get_byclasstopic</t>
   </si>
   <si>
@@ -295,9 +289,6 @@
     <t>Tamilab3</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
     <t>HTTP/1.1 404 Not Found</t>
   </si>
   <si>
@@ -466,11 +457,6 @@
     <t>TC_08_class_get</t>
   </si>
   <si>
-    <t xml:space="preserve">
-TC_10_class_get
-</t>
-  </si>
-  <si>
     <t>TC_11_class_get</t>
   </si>
   <si>
@@ -483,7 +469,292 @@
     <t>class_delete_byclassid</t>
   </si>
   <si>
-    <t>Tamil100</t>
+    <t>TC_02_class_del</t>
+  </si>
+  <si>
+    <t>/batchReco/123</t>
+  </si>
+  <si>
+    <t>invalidClassId</t>
+  </si>
+  <si>
+    <t>TC_03_class_del</t>
+  </si>
+  <si>
+    <t>TC_08_class_post</t>
+  </si>
+  <si>
+    <t>invalidurl</t>
+  </si>
+  <si>
+    <t>Tamil1000</t>
+  </si>
+  <si>
+    <t>TC_01_class_put</t>
+  </si>
+  <si>
+    <t>class_put_newclass</t>
+  </si>
+  <si>
+    <t>byinvalidClassId</t>
+  </si>
+  <si>
+    <t>byClassId</t>
+  </si>
+  <si>
+    <t>newTamila</t>
+  </si>
+  <si>
+    <t>TC_02_class_put</t>
+  </si>
+  <si>
+    <t>TC_03_class_put</t>
+  </si>
+  <si>
+    <t>getiing created with invalid topic</t>
+  </si>
+  <si>
+    <t>TC_04_class_put</t>
+  </si>
+  <si>
+    <t>newTamila@</t>
+  </si>
+  <si>
+    <t>TC_05_class_put</t>
+  </si>
+  <si>
+    <t>Invalid Topic</t>
+  </si>
+  <si>
+    <t>***%%$$##</t>
+  </si>
+  <si>
+    <t>getiing updated with invalid topic</t>
+  </si>
+  <si>
+    <t>giving 401</t>
+  </si>
+  <si>
+    <t>TC_06_class_put</t>
+  </si>
+  <si>
+    <t>TC_07_class_put</t>
+  </si>
+  <si>
+    <t>DeletedBatchId</t>
+  </si>
+  <si>
+    <t>Tamil95</t>
+  </si>
+  <si>
+    <t>TC_08_class_put</t>
+  </si>
+  <si>
+    <t>getting 404</t>
+  </si>
+  <si>
+    <t>InvalidData</t>
+  </si>
+  <si>
+    <t>invalidData</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>validclassrecord</t>
+  </si>
+  <si>
+    <t>D:/Recordings</t>
+  </si>
+  <si>
+    <t>class_put_class_recording_path</t>
+  </si>
+  <si>
+    <t>TC_09_classAllRecord_put</t>
+  </si>
+  <si>
+    <t>TC_10_classAllRecord_put</t>
+  </si>
+  <si>
+    <t>TC_11_classAllRecord_put</t>
+  </si>
+  <si>
+    <t>$$$%%</t>
+  </si>
+  <si>
+    <t>getting 200 and update is happenning</t>
+  </si>
+  <si>
+    <t>TC_12_classAllRecord_put</t>
+  </si>
+  <si>
+    <t>invalidmethod</t>
+  </si>
+  <si>
+    <t>TC_13_classAllRecord_put</t>
+  </si>
+  <si>
+    <t>TC_01_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_02_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_03_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_04_class_noAuth</t>
+  </si>
+  <si>
+    <t>byinvalidTopic</t>
+  </si>
+  <si>
+    <t>Http</t>
+  </si>
+  <si>
+    <t>TC_10_class_get</t>
+  </si>
+  <si>
+    <t>TC_12_class_get</t>
+  </si>
+  <si>
+    <t>class_get_classdetails_byclassid</t>
+  </si>
+  <si>
+    <t>TC_13_class_get</t>
+  </si>
+  <si>
+    <t>class_get_allclasses_bybatchid</t>
+  </si>
+  <si>
+    <t>byStaffId</t>
+  </si>
+  <si>
+    <t>TC_14_class_get</t>
+  </si>
+  <si>
+    <t>class_get_allclasses_bystaffid</t>
+  </si>
+  <si>
+    <t>TC_15_class_get</t>
+  </si>
+  <si>
+    <t>class_get_allrecordings</t>
+  </si>
+  <si>
+    <t>TC_16_class_get</t>
+  </si>
+  <si>
+    <t>class_get_classrecordings_byclassid</t>
+  </si>
+  <si>
+    <t>TC_17_class_get</t>
+  </si>
+  <si>
+    <t>TC_18_class_get</t>
+  </si>
+  <si>
+    <t>TC_19_class_get</t>
+  </si>
+  <si>
+    <t>TC_20_class_get</t>
+  </si>
+  <si>
+    <t>TC_21_class_get</t>
+  </si>
+  <si>
+    <t>TC_22_class_get</t>
+  </si>
+  <si>
+    <t>byinvalidStaffId</t>
+  </si>
+  <si>
+    <t>TC_23_class_get</t>
+  </si>
+  <si>
+    <t>TC_24_class_get</t>
+  </si>
+  <si>
+    <t>TC_25_class_get</t>
+  </si>
+  <si>
+    <t>TC_26_class_get</t>
+  </si>
+  <si>
+    <t>TC_27_class_get</t>
+  </si>
+  <si>
+    <t>TC_28_class_get</t>
+  </si>
+  <si>
+    <t>TC_29_class_get</t>
+  </si>
+  <si>
+    <t>TC_30_class_get</t>
+  </si>
+  <si>
+    <t>kinh7</t>
+  </si>
+  <si>
+    <t>TC_05_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_06_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_07_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_08_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_09_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_01_class_InvalidURL</t>
+  </si>
+  <si>
+    <t>TC_10_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_11_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_12_class_noAuth</t>
+  </si>
+  <si>
+    <t>TC_01_class_chaining</t>
+  </si>
+  <si>
+    <t>C:/Ela/Recordings</t>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>TC_01_logout</t>
+  </si>
+  <si>
+    <t>logout</t>
+  </si>
+  <si>
+    <t>TC_02_logout</t>
+  </si>
+  <si>
+    <t>Logout successful</t>
+  </si>
+  <si>
+    <t>TC_01_logout_noauth</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Tamil94</t>
+  </si>
+  <si>
+    <t>*&amp;^^$TY^&amp;</t>
   </si>
 </sst>
 </file>
@@ -646,7 +917,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -828,13 +1099,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1015,7 +1292,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1032,8 +1309,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1062,9 +1338,12 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1441,27 +1720,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.59765625" customWidth="1"/>
-    <col min="4" max="4" width="26.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.296875" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.09765625" customWidth="1"/>
-    <col min="12" max="12" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="14.59765625" customWidth="1"/>
+    <col min="6" max="6" width="26.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.296875" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.09765625" customWidth="1"/>
+    <col min="14" max="14" width="14.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1472,25 +1751,31 @@
         <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="K1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1500,17 +1785,23 @@
       <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="s">
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>234</v>
+      </c>
+      <c r="H2" t="s">
         <v>59</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>200</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="27.6">
+    <row r="3" spans="1:11" s="2" customFormat="1">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1520,132 +1811,237 @@
       <c r="C3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G3" s="5">
+      <c r="I3" s="5">
         <v>400</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" s="11" customFormat="1" ht="41.4">
-      <c r="A4" s="11" t="s">
+      <c r="K3" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="10" customFormat="1" ht="41.4">
+      <c r="A4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="G4" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="11">
+      <c r="I4" s="10">
         <v>400</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="10" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
+      <c r="K4" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="23" t="s">
         <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" t="s">
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>234</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" t="s">
         <v>18</v>
       </c>
-      <c r="G5">
-        <v>401</v>
-      </c>
-      <c r="H5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+      <c r="I5">
+        <v>404</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>234</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="5">
+      <c r="I6" s="5">
         <v>400</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+      <c r="K6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="1"/>
-      <c r="G7" s="5">
+      <c r="G7" s="1"/>
+      <c r="I7" s="5">
         <v>400</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="J7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>101</v>
+      <c r="K7" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>236</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9">
+        <v>404</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" t="s">
+        <v>237</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" t="s">
+        <v>236</v>
+      </c>
+      <c r="I10">
+        <v>200</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" t="s">
+        <v>239</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
+        <v>240</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" t="s">
+        <v>236</v>
+      </c>
+      <c r="I11">
+        <v>401</v>
+      </c>
+      <c r="J11" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4" display="March@"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="F3" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
+    <hyperlink ref="F4" r:id="rId3"/>
+    <hyperlink ref="G4" r:id="rId4" display="March@"/>
+    <hyperlink ref="G6" r:id="rId5"/>
+    <hyperlink ref="F7" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
@@ -1657,7 +2053,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1748,7 +2144,7 @@
         <v>37</v>
       </c>
       <c r="G3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H3">
         <v>201</v>
@@ -1813,144 +2209,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H1" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="I1" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="J1" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="L1" s="13" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="N1" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="O1" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="P1" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="Q1" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="R1" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="S1" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="T1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+    </row>
+    <row r="2" spans="1:26" s="10" customFormat="1" ht="28.2" thickBot="1">
+      <c r="A2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="F2" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="G2" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="T1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="U1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-    </row>
-    <row r="2" spans="1:26" s="11" customFormat="1" ht="28.2" thickBot="1">
-      <c r="A2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="15" t="s">
+      <c r="H2" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="I2" s="14" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="J2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="K2" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="L2" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="M2" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="N2" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="O2" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="P2" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="R2" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="M2" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="P2" s="15" t="s">
+      <c r="S2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="S2" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="18">
+      <c r="T2" s="14"/>
+      <c r="U2" s="17">
         <v>201</v>
       </c>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
+      <c r="V2" s="14"/>
+      <c r="W2" s="14"/>
+      <c r="X2" s="14"/>
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1964,96 +2360,97 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W20"/>
+  <dimension ref="A1:X73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.69921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.09765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.69921875" customWidth="1"/>
+    <col min="3" max="3" width="7.19921875" style="20" customWidth="1"/>
+    <col min="4" max="4" width="31.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.8984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9.69921875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="55.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.69921875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="20.5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="17.296875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="29.19921875" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:24">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="20" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
         <v>53</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>61</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>64</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>40</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>42</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>62</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>45</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>46</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>65</v>
       </c>
-      <c r="R1" t="s">
-        <v>75</v>
-      </c>
       <c r="S1" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="T1" t="s">
         <v>1</v>
@@ -2067,130 +2464,133 @@
       <c r="W1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:23">
+      <c r="X1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>54</v>
       </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="G2">
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2">
         <v>2</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>48</v>
       </c>
-      <c r="I2" t="s">
-        <v>151</v>
-      </c>
       <c r="J2" t="s">
+        <v>241</v>
+      </c>
+      <c r="K2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="L2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" t="s">
         <v>49</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>50</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>51</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>52</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>63</v>
       </c>
       <c r="U2">
         <v>201</v>
       </c>
       <c r="V2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>54</v>
       </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="G3">
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3">
         <v>2</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>48</v>
       </c>
-      <c r="I3" t="s">
-        <v>88</v>
-      </c>
       <c r="J3" t="s">
+        <v>86</v>
+      </c>
+      <c r="K3" t="s">
         <v>37</v>
       </c>
-      <c r="K3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="L3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" t="s">
         <v>66</v>
       </c>
       <c r="U3">
         <v>201</v>
       </c>
       <c r="V3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>54</v>
       </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="K4" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="N4" t="s">
         <v>56</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>50</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>51</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>52</v>
       </c>
       <c r="U4">
@@ -2200,50 +2600,50 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="8" t="s">
-        <v>133</v>
+    <row r="5" spans="1:24">
+      <c r="A5" s="23" t="s">
+        <v>130</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
+        <v>176</v>
+      </c>
+      <c r="D5" t="s">
         <v>54</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="G5">
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5">
         <v>2</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>48</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>89</v>
-      </c>
       <c r="J5" t="s">
+        <v>242</v>
+      </c>
+      <c r="K5" t="s">
         <v>37</v>
       </c>
-      <c r="K5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="L5" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" t="s">
         <v>49</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>50</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>51</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>52</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>63</v>
       </c>
       <c r="U5">
@@ -2252,51 +2652,54 @@
       <c r="V5" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:23">
+      <c r="X5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" t="s">
         <v>54</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
       <c r="E6" t="s">
         <v>15</v>
       </c>
-      <c r="G6">
+      <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6">
         <v>2</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>48</v>
       </c>
-      <c r="I6" t="s">
-        <v>86</v>
-      </c>
       <c r="J6" t="s">
+        <v>84</v>
+      </c>
+      <c r="K6" t="s">
         <v>37</v>
       </c>
-      <c r="K6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M6" t="s">
+      <c r="L6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" t="s">
         <v>49</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>50</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>51</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>52</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>63</v>
       </c>
       <c r="U6">
@@ -2306,79 +2709,80 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:24">
       <c r="A7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" t="s">
         <v>54</v>
       </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
       <c r="E7" t="s">
         <v>15</v>
       </c>
-      <c r="G7">
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7">
         <v>2</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>48</v>
       </c>
-      <c r="I7" t="s">
-        <v>70</v>
-      </c>
       <c r="J7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" t="s">
         <v>37</v>
       </c>
-      <c r="K7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M7" t="s">
+      <c r="L7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" t="s">
         <v>49</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>50</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>51</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>52</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>63</v>
       </c>
       <c r="T7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="U7">
         <v>404</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:24">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
         <v>54</v>
       </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
       <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
         <v>13</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>13</v>
       </c>
       <c r="U8">
@@ -2388,272 +2792,1662 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
-      <c r="A9" t="s">
-        <v>137</v>
+    <row r="9" spans="1:24">
+      <c r="A9" s="21" t="s">
+        <v>151</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C9" t="s">
-        <v>73</v>
+        <v>15</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
-      </c>
-      <c r="U9">
+        <v>54</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="V9" s="2"/>
+    </row>
+    <row r="11" spans="1:24">
+      <c r="A11" s="20" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
+        <v>155</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H11">
+        <v>2</v>
+      </c>
+      <c r="I11" t="s">
+        <v>48</v>
+      </c>
+      <c r="J11" t="s">
+        <v>158</v>
+      </c>
+      <c r="K11" t="s">
+        <v>37</v>
+      </c>
+      <c r="L11" t="s">
+        <v>15</v>
+      </c>
+      <c r="R11" t="s">
+        <v>66</v>
+      </c>
+      <c r="U11">
         <v>200</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
-      <c r="A10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>15</v>
-      </c>
-      <c r="T10" t="s">
-        <v>69</v>
-      </c>
-      <c r="U10">
+    <row r="12" spans="1:24">
+      <c r="A12" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="B12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="S12">
+        <v>786543</v>
+      </c>
+      <c r="U12">
         <v>404</v>
       </c>
-      <c r="V10" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23">
-      <c r="A11" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
-      <c r="U11">
-        <v>405</v>
-      </c>
-      <c r="V11" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23">
-      <c r="A12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="U12">
-        <v>200</v>
-      </c>
-      <c r="V12" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23">
-      <c r="A13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" t="s">
-        <v>77</v>
+      <c r="V12" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:24">
+      <c r="A13" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="B13" t="s">
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13">
-        <v>12345</v>
+        <v>155</v>
+      </c>
+      <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" t="s">
+        <v>15</v>
+      </c>
+      <c r="N13" t="s">
+        <v>56</v>
+      </c>
+      <c r="O13" t="s">
+        <v>50</v>
+      </c>
+      <c r="P13" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>52</v>
       </c>
       <c r="U13">
+        <v>400</v>
+      </c>
+      <c r="V13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X13" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="14" spans="1:24">
+      <c r="A14" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="B14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>1223</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="K14" t="s">
+        <v>37</v>
+      </c>
+      <c r="L14" t="s">
+        <v>15</v>
+      </c>
+      <c r="N14" t="s">
+        <v>49</v>
+      </c>
+      <c r="O14" t="s">
+        <v>50</v>
+      </c>
+      <c r="P14" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>52</v>
+      </c>
+      <c r="R14" t="s">
+        <v>63</v>
+      </c>
+      <c r="U14">
+        <v>400</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:24">
+      <c r="A15" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B15" t="s">
+        <v>165</v>
+      </c>
+      <c r="D15" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15">
+        <v>2</v>
+      </c>
+      <c r="I15" t="s">
+        <v>48</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="K15" t="s">
+        <v>37</v>
+      </c>
+      <c r="L15" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" t="s">
+        <v>49</v>
+      </c>
+      <c r="O15" t="s">
+        <v>50</v>
+      </c>
+      <c r="P15" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>52</v>
+      </c>
+      <c r="R15" t="s">
+        <v>63</v>
+      </c>
+      <c r="U15">
+        <v>400</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="16" spans="1:24">
+      <c r="A16" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16">
+        <v>2</v>
+      </c>
+      <c r="I16" t="s">
+        <v>48</v>
+      </c>
+      <c r="J16" t="s">
+        <v>158</v>
+      </c>
+      <c r="K16" t="s">
+        <v>37</v>
+      </c>
+      <c r="L16" t="s">
+        <v>15</v>
+      </c>
+      <c r="R16" t="s">
+        <v>66</v>
+      </c>
+      <c r="T16" t="s">
+        <v>68</v>
+      </c>
+      <c r="U16">
         <v>404</v>
       </c>
-      <c r="V13" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23">
-      <c r="A14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C14" t="s">
-        <v>77</v>
-      </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="T14" t="s">
-        <v>79</v>
-      </c>
-      <c r="U14">
-        <v>404</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23">
-      <c r="A15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="C15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>15</v>
-      </c>
-      <c r="U15">
-        <v>405</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23">
-      <c r="A16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C16" t="s">
-        <v>82</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="S16" t="s">
-        <v>83</v>
-      </c>
-      <c r="U16">
-        <v>200</v>
-      </c>
-      <c r="V16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22">
-      <c r="A17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C17" t="s">
-        <v>82</v>
+      <c r="V16" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24">
+      <c r="A17" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" t="s">
+        <v>171</v>
       </c>
       <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="S17" t="s">
-        <v>84</v>
+        <v>155</v>
+      </c>
+      <c r="E17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17">
+        <v>9842</v>
+      </c>
+      <c r="H17">
+        <v>2</v>
+      </c>
+      <c r="I17" t="s">
+        <v>48</v>
+      </c>
+      <c r="J17" t="s">
+        <v>158</v>
+      </c>
+      <c r="K17" t="s">
+        <v>37</v>
+      </c>
+      <c r="L17" t="s">
+        <v>15</v>
+      </c>
+      <c r="R17" t="s">
+        <v>66</v>
+      </c>
+      <c r="S17">
+        <v>3066</v>
       </c>
       <c r="U17">
         <v>404</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" s="11" customFormat="1" ht="41.4">
-      <c r="A18" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="X17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:24">
+      <c r="A18" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="B18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D18" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="I18" t="s">
+        <v>48</v>
+      </c>
+      <c r="J18" t="s">
+        <v>158</v>
+      </c>
+      <c r="K18" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" t="s">
+        <v>15</v>
+      </c>
+      <c r="U18">
+        <v>404</v>
+      </c>
+      <c r="V18" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24">
+      <c r="A19" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" t="s">
+        <v>178</v>
+      </c>
+      <c r="D19" t="s">
+        <v>180</v>
+      </c>
+      <c r="E19" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>179</v>
+      </c>
+      <c r="U19">
+        <v>200</v>
+      </c>
+      <c r="V19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24">
+      <c r="A20" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" t="s">
+        <v>156</v>
+      </c>
+      <c r="D20" t="s">
+        <v>180</v>
+      </c>
+      <c r="E20" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>179</v>
+      </c>
+      <c r="S20">
+        <v>3066</v>
+      </c>
+      <c r="U20">
+        <v>404</v>
+      </c>
+      <c r="V20" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24">
+      <c r="A21" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="B21" t="s">
+        <v>176</v>
+      </c>
+      <c r="D21" t="s">
+        <v>180</v>
+      </c>
+      <c r="E21" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>184</v>
+      </c>
+      <c r="U21">
+        <v>400</v>
+      </c>
+      <c r="V21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24">
+      <c r="A22" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="B22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>179</v>
+      </c>
+      <c r="U22">
+        <v>405</v>
+      </c>
+      <c r="V22" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24">
+      <c r="A23" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" t="s">
+        <v>180</v>
+      </c>
+      <c r="E23" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>179</v>
+      </c>
+      <c r="U23">
+        <v>404</v>
+      </c>
+      <c r="V23" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24">
+      <c r="A24" s="20"/>
+      <c r="V24" s="2"/>
+    </row>
+    <row r="25" spans="1:24">
+      <c r="A25" t="s">
+        <v>134</v>
+      </c>
+      <c r="B25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+      <c r="U25">
+        <v>200</v>
+      </c>
+      <c r="V25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24">
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
+        <v>15</v>
+      </c>
+      <c r="T26" t="s">
+        <v>68</v>
+      </c>
+      <c r="U26">
+        <v>404</v>
+      </c>
+      <c r="V26" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24">
+      <c r="A27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+      <c r="U27">
+        <v>405</v>
+      </c>
+      <c r="V27" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24">
+      <c r="A28" t="s">
+        <v>137</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="7"/>
+      <c r="D28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E28" t="s">
+        <v>15</v>
+      </c>
+      <c r="U28">
+        <v>200</v>
+      </c>
+      <c r="V28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24">
+      <c r="A29" t="s">
+        <v>138</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+      <c r="E29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29">
+        <v>12345</v>
+      </c>
+      <c r="U29">
+        <v>404</v>
+      </c>
+      <c r="V29" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24">
+      <c r="A30" t="s">
+        <v>139</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" t="s">
+        <v>15</v>
+      </c>
+      <c r="T30" t="s">
+        <v>78</v>
+      </c>
+      <c r="U30">
+        <v>404</v>
+      </c>
+      <c r="V30" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24">
+      <c r="A31" t="s">
+        <v>140</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D31" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" t="s">
+        <v>15</v>
+      </c>
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+      <c r="U31">
+        <v>405</v>
+      </c>
+      <c r="V31" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24">
+      <c r="A32" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="7"/>
+      <c r="D32" t="s">
+        <v>80</v>
+      </c>
+      <c r="E32" t="s">
+        <v>15</v>
+      </c>
+      <c r="J32" t="s">
+        <v>81</v>
+      </c>
+      <c r="U32">
+        <v>200</v>
+      </c>
+      <c r="V32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
+      <c r="A33" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C33" s="7"/>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" t="s">
+        <v>15</v>
+      </c>
+      <c r="J33" t="s">
+        <v>82</v>
+      </c>
+      <c r="U33">
+        <v>404</v>
+      </c>
+      <c r="V33" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" s="6" customFormat="1" ht="15" customHeight="1">
+      <c r="A34" t="s">
+        <v>195</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>80</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="U34">
+        <v>405</v>
+      </c>
+      <c r="V34" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22">
+      <c r="A35" t="s">
+        <v>143</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="D35" t="s">
+        <v>80</v>
+      </c>
+      <c r="E35" t="s">
+        <v>15</v>
+      </c>
+      <c r="T35" t="s">
+        <v>89</v>
+      </c>
+      <c r="U35">
+        <v>404</v>
+      </c>
+      <c r="V35" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22">
+      <c r="A36" t="s">
+        <v>196</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C36" s="7"/>
+      <c r="D36" t="s">
+        <v>197</v>
+      </c>
+      <c r="E36" t="s">
+        <v>15</v>
+      </c>
+      <c r="U36">
+        <v>200</v>
+      </c>
+      <c r="V36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:22">
+      <c r="A37" t="s">
+        <v>198</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" t="s">
+        <v>199</v>
+      </c>
+      <c r="E37" t="s">
+        <v>15</v>
+      </c>
+      <c r="U37">
+        <v>200</v>
+      </c>
+      <c r="V37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22">
+      <c r="A38" t="s">
+        <v>201</v>
+      </c>
+      <c r="B38" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" t="s">
+        <v>202</v>
+      </c>
+      <c r="E38" t="s">
+        <v>15</v>
+      </c>
+      <c r="U38">
+        <v>200</v>
+      </c>
+      <c r="V38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:22">
+      <c r="A39" t="s">
+        <v>203</v>
+      </c>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" t="s">
+        <v>204</v>
+      </c>
+      <c r="E39" t="s">
+        <v>15</v>
+      </c>
+      <c r="U39">
+        <v>200</v>
+      </c>
+      <c r="V39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:22">
+      <c r="A40" t="s">
+        <v>205</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C40" s="7"/>
+      <c r="D40" t="s">
+        <v>206</v>
+      </c>
+      <c r="E40" t="s">
+        <v>15</v>
+      </c>
+      <c r="U40">
+        <v>200</v>
+      </c>
+      <c r="V40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:22">
+      <c r="A41" t="s">
+        <v>207</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C41" s="7"/>
+      <c r="D41" t="s">
+        <v>197</v>
+      </c>
+      <c r="E41" t="s">
+        <v>15</v>
+      </c>
+      <c r="S41">
+        <v>12345</v>
+      </c>
+      <c r="U41">
+        <v>404</v>
+      </c>
+      <c r="V41" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:22">
+      <c r="A42" t="s">
+        <v>208</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" t="s">
+        <v>197</v>
+      </c>
+      <c r="E42" t="s">
+        <v>15</v>
+      </c>
+      <c r="T42" t="s">
+        <v>89</v>
+      </c>
+      <c r="U42">
+        <v>404</v>
+      </c>
+      <c r="V42" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:22">
+      <c r="A43" t="s">
+        <v>209</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D43" t="s">
+        <v>197</v>
+      </c>
+      <c r="E43" t="s">
+        <v>15</v>
+      </c>
+      <c r="U43">
+        <v>405</v>
+      </c>
+      <c r="V43" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:22">
+      <c r="A44" t="s">
+        <v>210</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" t="s">
+        <v>202</v>
+      </c>
+      <c r="E44" t="s">
+        <v>15</v>
+      </c>
+      <c r="U44">
+        <v>404</v>
+      </c>
+      <c r="V44" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22">
+      <c r="A45" t="s">
+        <v>211</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" t="s">
+        <v>202</v>
+      </c>
+      <c r="E45" t="s">
+        <v>15</v>
+      </c>
+      <c r="M45">
+        <v>8766</v>
+      </c>
+      <c r="U45">
+        <v>404</v>
+      </c>
+      <c r="V45" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:22">
+      <c r="A46" t="s">
+        <v>212</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="C46" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D46" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="E46" t="s">
+        <v>15</v>
+      </c>
+      <c r="U46">
+        <v>405</v>
+      </c>
+      <c r="V46" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22">
+      <c r="A47" t="s">
+        <v>214</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" s="7"/>
+      <c r="D47" t="s">
+        <v>199</v>
+      </c>
+      <c r="E47" t="s">
+        <v>15</v>
+      </c>
+      <c r="U47">
+        <v>404</v>
+      </c>
+      <c r="V47" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:22">
+      <c r="A48" t="s">
+        <v>215</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="C48" s="7"/>
+      <c r="D48" t="s">
+        <v>199</v>
+      </c>
+      <c r="E48" t="s">
+        <v>15</v>
+      </c>
+      <c r="G48">
+        <v>456</v>
+      </c>
+      <c r="T48" t="s">
+        <v>89</v>
+      </c>
+      <c r="U48">
+        <v>404</v>
+      </c>
+      <c r="V48" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22">
+      <c r="A49" t="s">
+        <v>216</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D49" t="s">
+        <v>199</v>
+      </c>
+      <c r="E49" t="s">
+        <v>15</v>
+      </c>
+      <c r="U49">
+        <v>405</v>
+      </c>
+      <c r="V49" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22">
+      <c r="A50" t="s">
+        <v>217</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="7"/>
+      <c r="D50" t="s">
+        <v>204</v>
+      </c>
+      <c r="E50" t="s">
+        <v>15</v>
+      </c>
+      <c r="T50" t="s">
+        <v>148</v>
+      </c>
+      <c r="U50">
+        <v>404</v>
+      </c>
+      <c r="V50" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="51" spans="1:22">
+      <c r="A51" t="s">
+        <v>218</v>
+      </c>
+      <c r="B51" s="7"/>
+      <c r="C51" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" t="s">
+        <v>204</v>
+      </c>
+      <c r="E51" t="s">
+        <v>15</v>
+      </c>
+      <c r="U51">
+        <v>405</v>
+      </c>
+      <c r="V51" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:22">
+      <c r="A52" t="s">
+        <v>219</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C52" s="7"/>
+      <c r="D52" t="s">
+        <v>206</v>
+      </c>
+      <c r="E52" t="s">
+        <v>15</v>
+      </c>
+      <c r="S52" t="s">
+        <v>222</v>
+      </c>
+      <c r="U52">
+        <v>404</v>
+      </c>
+      <c r="V52" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22">
+      <c r="A53" t="s">
+        <v>220</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="7"/>
+      <c r="D53" t="s">
+        <v>206</v>
+      </c>
+      <c r="E53" t="s">
+        <v>15</v>
+      </c>
+      <c r="U53">
+        <v>404</v>
+      </c>
+      <c r="V53" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="54" spans="1:22">
+      <c r="A54" t="s">
+        <v>221</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C54" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D54" t="s">
+        <v>206</v>
+      </c>
+      <c r="E54" t="s">
+        <v>15</v>
+      </c>
+      <c r="U54">
+        <v>405</v>
+      </c>
+      <c r="V54" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22">
+      <c r="A55" t="s">
+        <v>144</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C55" s="7"/>
+      <c r="D55" t="s">
         <v>146</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="E55" t="s">
+        <v>15</v>
+      </c>
+      <c r="U55">
+        <v>200</v>
+      </c>
+      <c r="V55" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22">
+      <c r="A56" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="7"/>
+      <c r="D56" t="s">
+        <v>146</v>
+      </c>
+      <c r="E56" t="s">
+        <v>15</v>
+      </c>
+      <c r="T56" t="s">
+        <v>148</v>
+      </c>
+      <c r="U56">
+        <v>404</v>
+      </c>
+      <c r="V56" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22">
+      <c r="A57" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="C57" s="7"/>
+      <c r="D57" t="s">
+        <v>146</v>
+      </c>
+      <c r="E57" t="s">
+        <v>15</v>
+      </c>
+      <c r="S57">
+        <v>123</v>
+      </c>
+      <c r="U57">
+        <v>404</v>
+      </c>
+      <c r="V57" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22">
+      <c r="B58" s="19"/>
+      <c r="C58" s="7"/>
+      <c r="V58" s="2"/>
+    </row>
+    <row r="59" spans="1:22">
+      <c r="A59" t="s">
+        <v>189</v>
+      </c>
+      <c r="B59" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" t="s">
+        <v>54</v>
+      </c>
+      <c r="E59" t="s">
+        <v>13</v>
+      </c>
+      <c r="F59" t="s">
+        <v>15</v>
+      </c>
+      <c r="H59">
+        <v>2</v>
+      </c>
+      <c r="I59" t="s">
+        <v>48</v>
+      </c>
+      <c r="J59" t="s">
+        <v>172</v>
+      </c>
+      <c r="K59" t="s">
+        <v>37</v>
+      </c>
+      <c r="L59" t="s">
+        <v>15</v>
+      </c>
+      <c r="N59" t="s">
+        <v>49</v>
+      </c>
+      <c r="O59" t="s">
+        <v>50</v>
+      </c>
+      <c r="P59" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>52</v>
+      </c>
+      <c r="R59" t="s">
+        <v>63</v>
+      </c>
+      <c r="U59">
+        <v>401</v>
+      </c>
+      <c r="V59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:22">
+      <c r="A60" t="s">
+        <v>190</v>
+      </c>
+      <c r="B60" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" t="s">
+        <v>72</v>
+      </c>
+      <c r="E60" t="s">
+        <v>13</v>
+      </c>
+      <c r="U60">
+        <v>401</v>
+      </c>
+      <c r="V60" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="61" spans="1:22">
+      <c r="A61" t="s">
+        <v>191</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C61" s="7"/>
+      <c r="D61" t="s">
+        <v>76</v>
+      </c>
+      <c r="E61" t="s">
+        <v>13</v>
+      </c>
+      <c r="U61">
+        <v>401</v>
+      </c>
+      <c r="V61" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="62" spans="1:22">
+      <c r="A62" t="s">
+        <v>192</v>
+      </c>
+      <c r="B62" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" s="7"/>
+      <c r="D62" t="s">
+        <v>197</v>
+      </c>
+      <c r="E62" t="s">
+        <v>13</v>
+      </c>
+      <c r="U62">
+        <v>401</v>
+      </c>
+      <c r="V62" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="1:22">
+      <c r="A63" t="s">
+        <v>223</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="7"/>
+      <c r="D63" t="s">
+        <v>199</v>
+      </c>
+      <c r="E63" t="s">
+        <v>13</v>
+      </c>
+      <c r="U63">
+        <v>401</v>
+      </c>
+      <c r="V63" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22">
+      <c r="A64" t="s">
+        <v>224</v>
+      </c>
+      <c r="B64" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="D64" t="s">
+        <v>202</v>
+      </c>
+      <c r="E64" t="s">
+        <v>13</v>
+      </c>
+      <c r="U64">
+        <v>401</v>
+      </c>
+      <c r="V64" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22">
+      <c r="A65" t="s">
+        <v>225</v>
+      </c>
+      <c r="D65" t="s">
+        <v>204</v>
+      </c>
+      <c r="E65" t="s">
+        <v>13</v>
+      </c>
+      <c r="U65">
+        <v>401</v>
+      </c>
+      <c r="V65" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22">
+      <c r="A66" t="s">
+        <v>226</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C66" s="7"/>
+      <c r="D66" t="s">
+        <v>206</v>
+      </c>
+      <c r="E66" t="s">
+        <v>13</v>
+      </c>
+      <c r="U66">
+        <v>401</v>
+      </c>
+      <c r="V66" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22">
+      <c r="A67" t="s">
+        <v>227</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="C67" s="7"/>
+      <c r="D67" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="S18" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="U18" s="11">
-        <v>405</v>
-      </c>
-      <c r="V18" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22">
-      <c r="A19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" t="s">
-        <v>82</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="T19" t="s">
-        <v>92</v>
-      </c>
-      <c r="U19">
+      <c r="E67" t="s">
+        <v>13</v>
+      </c>
+      <c r="J67" t="s">
+        <v>172</v>
+      </c>
+      <c r="U67">
+        <v>401</v>
+      </c>
+      <c r="V67" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="68" spans="1:22">
+      <c r="A68" t="s">
+        <v>229</v>
+      </c>
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" t="s">
+        <v>155</v>
+      </c>
+      <c r="E68" t="s">
+        <v>13</v>
+      </c>
+      <c r="F68" t="s">
+        <v>15</v>
+      </c>
+      <c r="H68">
+        <v>2</v>
+      </c>
+      <c r="I68" t="s">
+        <v>48</v>
+      </c>
+      <c r="J68" t="s">
+        <v>158</v>
+      </c>
+      <c r="K68" t="s">
+        <v>37</v>
+      </c>
+      <c r="L68" t="s">
+        <v>15</v>
+      </c>
+      <c r="R68" t="s">
+        <v>66</v>
+      </c>
+      <c r="U68">
+        <v>401</v>
+      </c>
+      <c r="V68" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="69" spans="1:22">
+      <c r="A69" t="s">
+        <v>230</v>
+      </c>
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" t="s">
+        <v>180</v>
+      </c>
+      <c r="E69" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>179</v>
+      </c>
+      <c r="U69">
+        <v>401</v>
+      </c>
+      <c r="V69" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="70" spans="1:22">
+      <c r="A70" t="s">
+        <v>231</v>
+      </c>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" t="s">
+        <v>146</v>
+      </c>
+      <c r="E70" t="s">
+        <v>13</v>
+      </c>
+      <c r="U70">
+        <v>401</v>
+      </c>
+      <c r="V70" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="71" spans="1:22">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+    </row>
+    <row r="72" spans="1:22">
+      <c r="A72" s="21" t="s">
+        <v>228</v>
+      </c>
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" t="s">
+        <v>54</v>
+      </c>
+      <c r="E72" t="s">
+        <v>152</v>
+      </c>
+      <c r="F72" t="s">
+        <v>15</v>
+      </c>
+      <c r="H72">
+        <v>2</v>
+      </c>
+      <c r="I72" t="s">
+        <v>48</v>
+      </c>
+      <c r="J72" t="s">
+        <v>153</v>
+      </c>
+      <c r="K72" t="s">
+        <v>37</v>
+      </c>
+      <c r="L72" t="s">
+        <v>15</v>
+      </c>
+      <c r="N72" t="s">
+        <v>49</v>
+      </c>
+      <c r="O72" t="s">
+        <v>50</v>
+      </c>
+      <c r="P72" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q72" t="s">
+        <v>52</v>
+      </c>
+      <c r="R72" t="s">
+        <v>63</v>
+      </c>
+      <c r="U72">
         <v>404</v>
       </c>
-      <c r="V19" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22">
-      <c r="A20" t="s">
-        <v>148</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>149</v>
-      </c>
-      <c r="C20" t="s">
-        <v>150</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="U20">
+      <c r="V72" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22">
+      <c r="A73" t="s">
+        <v>232</v>
+      </c>
+      <c r="B73" t="s">
+        <v>57</v>
+      </c>
+      <c r="D73" t="s">
+        <v>155</v>
+      </c>
+      <c r="E73" t="s">
+        <v>15</v>
+      </c>
+      <c r="F73" t="s">
+        <v>15</v>
+      </c>
+      <c r="H73">
+        <v>2</v>
+      </c>
+      <c r="I73" t="s">
+        <v>48</v>
+      </c>
+      <c r="J73" t="s">
+        <v>158</v>
+      </c>
+      <c r="K73" t="s">
+        <v>37</v>
+      </c>
+      <c r="L73" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q73" t="s">
+        <v>233</v>
+      </c>
+      <c r="R73" t="s">
+        <v>66</v>
+      </c>
+      <c r="U73">
         <v>200</v>
       </c>
-      <c r="V20" t="s">
+      <c r="V73" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J14" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
User Module Test Data
</commit_message>
<xml_diff>
--- a/Team04_RestfulRebels/src/test/resources/TestData/Team04_RestfulRebels.xlsx
+++ b/Team04_RestfulRebels/src/test/resources/TestData/Team04_RestfulRebels.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ems11\Desktop\ElamathiProjects\Team04_RestfulRebels_APIPhase2\Team04_RestfulRebels\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shruti/new_eclipseWorkspace/Team04_RestfulRebels_APIPhase2/Team04_RestfulRebels/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F913BE92-F97F-4144-B63B-19F3EB54AB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="234">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -382,15 +383,6 @@
     <t>NN Users of SDET</t>
   </si>
   <si>
-    <t>B.E</t>
-  </si>
-  <si>
-    <t>M.S</t>
-  </si>
-  <si>
-    <t>TeamFour</t>
-  </si>
-  <si>
     <t>RestAssured</t>
   </si>
   <si>
@@ -410,12 +402,6 @@
   </si>
   <si>
     <t>R03</t>
-  </si>
-  <si>
-    <t>nnteam5@gmail.com</t>
-  </si>
-  <si>
-    <t>+91 1016213107</t>
   </si>
   <si>
     <t>TC_01_class_post</t>
@@ -484,13 +470,274 @@
   </si>
   <si>
     <t>Tamil100</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>RestfulRebels</t>
+  </si>
+  <si>
+    <t>Rebels</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>TEAM 4 Users</t>
+  </si>
+  <si>
+    <t>RebelsTeamUser</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/RestfulRebels4455</t>
+  </si>
+  <si>
+    <t>Austin</t>
+  </si>
+  <si>
+    <t>Numpy</t>
+  </si>
+  <si>
+    <t>www.linkedin@com/RestfulRebels12</t>
+  </si>
+  <si>
+    <t>H1B</t>
+  </si>
+  <si>
+    <t>team4restfulrebels444@gmail.com</t>
+  </si>
+  <si>
+    <t>Exisitng</t>
+  </si>
+  <si>
+    <t>RestfulRebelsTeamShruti</t>
+  </si>
+  <si>
+    <t>www.linkedin.com/RestfulRebels12</t>
+  </si>
+  <si>
+    <t>+91 1996213307</t>
+  </si>
+  <si>
+    <t>+91 5098883331</t>
+  </si>
+  <si>
+    <t>RestfulRebelsTeamfourUsr</t>
+  </si>
+  <si>
+    <t>BE</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
+    <t>team4rest@gmail.com</t>
+  </si>
+  <si>
+    <t>H4-EAD</t>
+  </si>
+  <si>
+    <t>+91 9191919191</t>
+  </si>
+  <si>
+    <t>JJ</t>
+  </si>
+  <si>
+    <t>12RestfulRebelsTeamShruti2234</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>DC</t>
+  </si>
+  <si>
+    <t>get_all_users</t>
+  </si>
+  <si>
+    <t>TC_07_user</t>
+  </si>
+  <si>
+    <t>get_all_active_users</t>
+  </si>
+  <si>
+    <t>TC_10_user</t>
+  </si>
+  <si>
+    <t>TC_08_user</t>
+  </si>
+  <si>
+    <t>TC_09_user</t>
+  </si>
+  <si>
+    <t>TC_11_user</t>
+  </si>
+  <si>
+    <t>get_all_userswithroles</t>
+  </si>
+  <si>
+    <t>get_userinformation_byuserid</t>
+  </si>
+  <si>
+    <t>get_emailsof_alluserswith_activestatus</t>
+  </si>
+  <si>
+    <t>TC_12_user</t>
+  </si>
+  <si>
+    <t>TC_13_user</t>
+  </si>
+  <si>
+    <t>TC_14_user</t>
+  </si>
+  <si>
+    <t>TC_15_user</t>
+  </si>
+  <si>
+    <t>TC_16_user</t>
+  </si>
+  <si>
+    <t>TC_17_user</t>
+  </si>
+  <si>
+    <t>get_allroles</t>
+  </si>
+  <si>
+    <t>get_countof_active_and_inactiveusers</t>
+  </si>
+  <si>
+    <t>get_userby_programbatches</t>
+  </si>
+  <si>
+    <t>get_usersfor_program</t>
+  </si>
+  <si>
+    <t>get_userby_roleid</t>
+  </si>
+  <si>
+    <t>get_userbyroleid_v2</t>
+  </si>
+  <si>
+    <t>put_byuserid</t>
+  </si>
+  <si>
+    <t>NN Users of Tech SDET</t>
+  </si>
+  <si>
+    <t>Kitss</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>+91 1996219999</t>
+  </si>
+  <si>
+    <t>TestUpdateTeamonetw</t>
+  </si>
+  <si>
+    <t>nntfourfour33323j@gmail.com</t>
+  </si>
+  <si>
+    <t>TC_18_user</t>
+  </si>
+  <si>
+    <t>invalid userId</t>
+  </si>
+  <si>
+    <t>NNNGFHASJ</t>
+  </si>
+  <si>
+    <t>SHHHHH</t>
+  </si>
+  <si>
+    <t>DD</t>
+  </si>
+  <si>
+    <t>+91 2233445566</t>
+  </si>
+  <si>
+    <t>TC_19_user</t>
+  </si>
+  <si>
+    <t>invalid-missing required field</t>
+  </si>
+  <si>
+    <t>sdfdsf</t>
+  </si>
+  <si>
+    <t>ff</t>
+  </si>
+  <si>
+    <t>put_byroleid</t>
+  </si>
+  <si>
+    <t>TC_20_user</t>
+  </si>
+  <si>
+    <t>TC_21_user</t>
+  </si>
+  <si>
+    <t>put_byuserrolepgmbatchstatus</t>
+  </si>
+  <si>
+    <t>userRoleProgramBatchStatus</t>
+  </si>
+  <si>
+    <t>byinvaliduserId</t>
+  </si>
+  <si>
+    <t>TC_22_user</t>
+  </si>
+  <si>
+    <t>validuserId</t>
+  </si>
+  <si>
+    <t>TC_23_user</t>
+  </si>
+  <si>
+    <t>missingfield</t>
+  </si>
+  <si>
+    <t>deletebyvaliduserId</t>
+  </si>
+  <si>
+    <t>TC_02_user_del</t>
+  </si>
+  <si>
+    <t>TC_01_user_del</t>
+  </si>
+  <si>
+    <t>deletebyinvaliduserId</t>
+  </si>
+  <si>
+    <t>deletebyuserid</t>
+  </si>
+  <si>
+    <t>+91 8011912302</t>
+  </si>
+  <si>
+    <t>nn3tfourfour35523j@gmail.com</t>
+  </si>
+  <si>
+    <t>+91 1134441110</t>
+  </si>
+  <si>
+    <t>team4restfulrebelsagain55@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -643,6 +890,36 @@
       <sz val="11"/>
       <color rgb="FF4EA72E"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF339966"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFB0207"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1015,7 +1292,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1030,10 +1307,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1046,7 +1321,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1062,9 +1337,14 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1440,28 +1720,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.59765625" customWidth="1"/>
-    <col min="4" max="4" width="26.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.296875" customWidth="1"/>
-    <col min="6" max="6" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.09765625" customWidth="1"/>
-    <col min="12" max="12" width="14.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.1640625" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1490,7 +1770,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1510,7 +1790,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="2" customFormat="1" ht="27.6">
+    <row r="3" spans="1:9" s="2" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1539,36 +1819,36 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="11" customFormat="1" ht="41.4">
-      <c r="A4" s="11" t="s">
+    <row r="4" spans="1:9" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>400</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1590,7 +1870,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1614,7 +1894,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -1634,18 +1914,18 @@
       <c r="H7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="8" t="s">
         <v>101</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D3" r:id="rId1"/>
-    <hyperlink ref="E3" r:id="rId2"/>
-    <hyperlink ref="D4" r:id="rId3"/>
-    <hyperlink ref="E4" r:id="rId4" display="March@"/>
-    <hyperlink ref="E6" r:id="rId5"/>
-    <hyperlink ref="D7" r:id="rId6"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E4" r:id="rId4" display="March@" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId7"/>
@@ -1653,27 +1933,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.3984375" customWidth="1"/>
-    <col min="7" max="7" width="11.296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1705,7 +1984,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -1728,7 +2007,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>27</v>
       </c>
@@ -1754,22 +2033,22 @@
         <v>201</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>31</v>
       </c>
@@ -1780,224 +2059,1035 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AA26"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.19921875" customWidth="1"/>
-    <col min="2" max="2" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.796875" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="26.1640625" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
     <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.296875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="18" customWidth="1"/>
+    <col min="22" max="22" width="16" customWidth="1"/>
+    <col min="23" max="23" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="6" customFormat="1" ht="14.4" thickBot="1">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:27" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="J1" s="14" t="s">
+      <c r="J1" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="N1" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="O1" s="14" t="s">
+      <c r="O1" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="14" t="s">
+      <c r="R1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="14" t="s">
+      <c r="S1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="T1" s="14" t="s">
+      <c r="T1" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="U1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="U1" s="14" t="s">
+      <c r="V1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="13" t="s">
+      <c r="W1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-    </row>
-    <row r="2" spans="1:26" s="11" customFormat="1" ht="28.2" thickBot="1">
-      <c r="A2" s="15" t="s">
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+    </row>
+    <row r="2" spans="1:27" s="9" customFormat="1" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="15" t="s">
+      <c r="D2" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="J2" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="L2" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="J2" s="17" t="s">
+      <c r="M2" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="N2" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="O2" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="P2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="16">
+        <v>201</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+    </row>
+    <row r="3" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K3" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="L3" s="20"/>
+      <c r="M3" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="N3" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="O3" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="P3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q3" s="20"/>
+      <c r="R3" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="S3" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="18"/>
+      <c r="U3" s="20"/>
+      <c r="V3" s="18">
+        <v>201</v>
+      </c>
+      <c r="W3" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="K4" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="N4" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>169</v>
+      </c>
+      <c r="P4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="R4" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="S4" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="T4" s="18"/>
+      <c r="U4" s="20"/>
+      <c r="V4" s="18">
+        <v>201</v>
+      </c>
+      <c r="W4" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>172</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="R5" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="S5" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="T5" s="20"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="20">
+        <v>400</v>
+      </c>
+      <c r="W5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>174</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="N6" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="O6" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q6" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="R6" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="S6" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="T6" s="18"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="18">
+        <v>400</v>
+      </c>
+      <c r="W6" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V7" s="18">
+        <v>200</v>
+      </c>
+      <c r="W7" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V8" s="18">
+        <v>200</v>
+      </c>
+      <c r="W8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V9" s="18">
+        <v>200</v>
+      </c>
+      <c r="W9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V10" s="18">
+        <v>200</v>
+      </c>
+      <c r="W10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V11" s="18">
+        <v>200</v>
+      </c>
+      <c r="W11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>182</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V12" s="18">
+        <v>200</v>
+      </c>
+      <c r="W12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V13" s="18">
+        <v>200</v>
+      </c>
+      <c r="W13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V14" s="18">
+        <v>200</v>
+      </c>
+      <c r="W14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V15" s="18">
+        <v>200</v>
+      </c>
+      <c r="W15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V16" s="18">
+        <v>200</v>
+      </c>
+      <c r="W16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="V17" s="18">
+        <v>200</v>
+      </c>
+      <c r="W17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="H18" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="I18" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="J18" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>202</v>
+      </c>
+      <c r="N18" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="O18" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="P18" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q18" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="V18" s="18">
+        <v>200</v>
+      </c>
+      <c r="W18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="I19" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>174</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="M19" s="22" t="s">
+        <v>210</v>
+      </c>
+      <c r="N19" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="O19" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="P19" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="V19" s="18">
+        <v>404</v>
+      </c>
+      <c r="W19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="B20" t="s">
+        <v>212</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K20" t="s">
+        <v>174</v>
+      </c>
+      <c r="L20" t="s">
+        <v>214</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="N20" t="s">
+        <v>150</v>
+      </c>
+      <c r="O20" t="s">
+        <v>123</v>
+      </c>
+      <c r="P20" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="S20" t="s">
+        <v>37</v>
+      </c>
+      <c r="V20" s="18">
+        <v>400</v>
+      </c>
+      <c r="W20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>215</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R21" t="s">
         <v>124</v>
       </c>
-      <c r="M2" s="19" t="s">
-        <v>129</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="O2" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="P2" s="15" t="s">
+      <c r="S21" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="R2" s="15" t="s">
-        <v>127</v>
-      </c>
-      <c r="S2" s="15" t="s">
+      <c r="V21" s="18">
+        <v>200</v>
+      </c>
+      <c r="W21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" t="s">
+        <v>222</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R22" t="s">
+        <v>147</v>
+      </c>
+      <c r="T22" t="s">
         <v>37</v>
       </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="18">
-        <v>201</v>
-      </c>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
+      <c r="V22" s="18">
+        <v>200</v>
+      </c>
+      <c r="W22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="B23" t="s">
+        <v>220</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="R23" t="s">
+        <v>147</v>
+      </c>
+      <c r="T23" t="s">
+        <v>37</v>
+      </c>
+      <c r="V23" s="18">
+        <v>404</v>
+      </c>
+      <c r="W23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B24" t="s">
+        <v>224</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="T24" t="s">
+        <v>37</v>
+      </c>
+      <c r="V24" s="18">
+        <v>400</v>
+      </c>
+      <c r="W24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" t="s">
+        <v>225</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="V25" s="18">
+        <v>200</v>
+      </c>
+      <c r="W25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B26" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>229</v>
+      </c>
+      <c r="V26" s="18">
+        <v>404</v>
+      </c>
+      <c r="W26" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="http://www.linkedin.com/"/>
-    <hyperlink ref="Q2" r:id="rId2"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="Q2" r:id="rId2" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="J4" r:id="rId3" display="http://www.linkedin.com/RestfulRebels4455" xr:uid="{7684B4DB-1979-9F4B-BFB9-C5C903B61A7F}"/>
+    <hyperlink ref="Q4" r:id="rId4" xr:uid="{9422EDE3-122F-C342-A8B9-EBBDAB5EE360}"/>
+    <hyperlink ref="J5" r:id="rId5" display="http://www.linkedin@com/RestfulRebels12" xr:uid="{EA3F0E8A-E6BD-AF4F-A212-6B7C320200DB}"/>
+    <hyperlink ref="J6" r:id="rId6" display="http://www.linkedin.com/RestfulRebels12" xr:uid="{255C721C-0BB0-BE40-8ED4-B38FF374AAF9}"/>
+    <hyperlink ref="Q6" r:id="rId7" display="mailto:team4restfulrebels444@gmail.com" xr:uid="{5038BB1D-8DD2-EB43-958F-B68C24A61EF1}"/>
+    <hyperlink ref="Q5" r:id="rId8" xr:uid="{B25024E8-8FC3-1B42-83E5-F71D2DC223D3}"/>
+    <hyperlink ref="J3" r:id="rId9" xr:uid="{7FFC137C-B525-564D-85EC-5DF246A1C928}"/>
+    <hyperlink ref="J18" r:id="rId10" xr:uid="{CE256CE3-D8B4-3643-B71F-4C9E659FD528}"/>
+    <hyperlink ref="Q18" r:id="rId11" xr:uid="{4B5F276F-5BB5-6D48-A870-F1860E5336C6}"/>
+    <hyperlink ref="J19" r:id="rId12" xr:uid="{943B6829-5D43-3243-A6CB-86717640835F}"/>
+    <hyperlink ref="Q19" r:id="rId13" xr:uid="{B8C4323B-4DAC-1342-A8B6-14A0E8F81545}"/>
+    <hyperlink ref="J20" r:id="rId14" xr:uid="{CCE5B004-2F3F-8D44-8458-EB003972622C}"/>
+    <hyperlink ref="Q20" r:id="rId15" xr:uid="{36CF06A9-79CB-3746-9FC3-21B539765B00}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId16"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H24" sqref="H24"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.8984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.09765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.69921875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.09765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="55.5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.69921875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.69921875" customWidth="1"/>
+    <col min="18" max="18" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" customWidth="1"/>
     <col min="20" max="20" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="29.19921875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="29.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2034,7 +3124,7 @@
       <c r="L1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" t="s">
         <v>44</v>
       </c>
       <c r="N1" t="s">
@@ -2068,9 +3158,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:23">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
@@ -2091,7 +3181,7 @@
         <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="J2" t="s">
         <v>37</v>
@@ -2121,9 +3211,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:23">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
@@ -2162,9 +3252,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:23">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
         <v>58</v>
@@ -2200,9 +3290,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:23">
-      <c r="A5" s="8" t="s">
-        <v>133</v>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>128</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
@@ -2253,9 +3343,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:23">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B6" t="s">
         <v>68</v>
@@ -2306,11 +3396,11 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:23">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C7" t="s">
@@ -2362,9 +3452,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:23">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B8" t="s">
         <v>72</v>
@@ -2388,9 +3478,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:23">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B9" t="s">
         <v>59</v>
@@ -2408,11 +3498,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:23">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>138</v>
-      </c>
-      <c r="B10" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C10" t="s">
@@ -2431,11 +3521,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="11" spans="1:23">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>139</v>
-      </c>
-      <c r="B11" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" t="s">
         <v>74</v>
       </c>
       <c r="C11" t="s">
@@ -2451,11 +3541,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:23">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>140</v>
-      </c>
-      <c r="B12" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12" t="s">
         <v>76</v>
       </c>
       <c r="C12" t="s">
@@ -2471,11 +3561,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:23">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>141</v>
-      </c>
-      <c r="B13" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B13" t="s">
         <v>78</v>
       </c>
       <c r="C13" t="s">
@@ -2494,11 +3584,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:23">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>142</v>
-      </c>
-      <c r="B14" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C14" t="s">
@@ -2517,11 +3607,11 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:23">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" t="s">
         <v>76</v>
       </c>
       <c r="C15" t="s">
@@ -2540,11 +3630,11 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:23">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B16" t="s">
         <v>80</v>
       </c>
       <c r="C16" t="s">
@@ -2563,11 +3653,11 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:22">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>144</v>
-      </c>
-      <c r="B17" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17" t="s">
         <v>80</v>
       </c>
       <c r="C17" t="s">
@@ -2586,34 +3676,34 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:22" s="11" customFormat="1" ht="41.4">
-      <c r="A18" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="B18" s="20" t="s">
+    <row r="18" spans="1:22" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="B18" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="S18" s="11" t="s">
+      <c r="D18" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="S18" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="U18" s="11">
+      <c r="U18" s="9">
         <v>405</v>
       </c>
       <c r="V18" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>147</v>
-      </c>
-      <c r="B19" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>71</v>
       </c>
       <c r="C19" t="s">
@@ -2632,15 +3722,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>148</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>149</v>
+        <v>143</v>
+      </c>
+      <c r="B20" t="s">
+        <v>144</v>
       </c>
       <c r="C20" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
pushing latest code to remote branch
</commit_message>
<xml_diff>
--- a/Team04_RestfulRebels/src/test/resources/TestData/Team04_RestfulRebels.xlsx
+++ b/Team04_RestfulRebels/src/test/resources/TestData/Team04_RestfulRebels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shruti/new_eclipseWorkspace/Team04_RestfulRebels_APIPhase2/Team04_RestfulRebels/src/test/resources/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F913BE92-F97F-4144-B63B-19F3EB54AB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A09593E-6DC2-0647-A76E-190CC32F2D3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20560" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -380,9 +380,6 @@
     <t>userRoleStatus</t>
   </si>
   <si>
-    <t>NN Users of SDET</t>
-  </si>
-  <si>
     <t>RestAssured</t>
   </si>
   <si>
@@ -721,16 +718,19 @@
     <t>deletebyuserid</t>
   </si>
   <si>
-    <t>+91 8011912302</t>
-  </si>
-  <si>
-    <t>nn3tfourfour35523j@gmail.com</t>
-  </si>
-  <si>
     <t>+91 1134441110</t>
   </si>
   <si>
     <t>team4restfulrebelsagain55@gmail.com</t>
+  </si>
+  <si>
+    <t>nnhhh</t>
+  </si>
+  <si>
+    <t>+91 9091912309</t>
+  </si>
+  <si>
+    <t>n3temfourfour35523j@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -2075,7 +2075,7 @@
   <dimension ref="A1:AA26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2155,7 +2155,7 @@
         <v>116</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="U1" s="12" t="s">
         <v>1</v>
@@ -2185,46 +2185,46 @@
         <v>15</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>166</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>203</v>
-      </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="K2" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="L2" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="M2" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="N2" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="M2" s="17" t="s">
-        <v>230</v>
-      </c>
-      <c r="N2" s="13" t="s">
+      <c r="O2" s="13" t="s">
         <v>122</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>123</v>
       </c>
       <c r="P2" s="13" t="s">
         <v>37</v>
       </c>
       <c r="Q2" s="15" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="R2" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S2" s="13" t="s">
         <v>37</v>
@@ -2259,33 +2259,33 @@
       <c r="F3" s="20"/>
       <c r="G3" s="20"/>
       <c r="H3" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="I3" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="I3" s="18" t="s">
-        <v>149</v>
-      </c>
       <c r="J3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K3" s="20" t="s">
         <v>119</v>
-      </c>
-      <c r="K3" s="20" t="s">
-        <v>120</v>
       </c>
       <c r="L3" s="20"/>
       <c r="M3" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="N3" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O3" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P3" s="18" t="s">
         <v>37</v>
       </c>
       <c r="Q3" s="20"/>
       <c r="R3" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S3" s="18" t="s">
         <v>37</v>
@@ -2313,46 +2313,46 @@
         <v>15</v>
       </c>
       <c r="E4" s="18" t="s">
+        <v>151</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="I4" s="18" t="s">
         <v>152</v>
       </c>
-      <c r="F4" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="I4" s="18" t="s">
+      <c r="J4" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="18" t="s">
         <v>154</v>
       </c>
-      <c r="K4" s="18" t="s">
+      <c r="L4" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="L4" s="18" t="s">
-        <v>156</v>
-      </c>
       <c r="M4" s="22" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="N4" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O4" s="18" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P4" s="18" t="s">
         <v>37</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="R4" s="18" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="S4" s="18" t="s">
         <v>37</v>
@@ -2380,46 +2380,46 @@
         <v>15</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F5" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="G5" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="G5" s="20" t="s">
-        <v>167</v>
-      </c>
       <c r="H5" s="18" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="I5" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>170</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="N5" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="K5" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="L5" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="M5" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="N5" s="18" t="s">
-        <v>150</v>
-      </c>
       <c r="O5" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="R5" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S5" s="20" t="s">
         <v>37</v>
@@ -2438,7 +2438,7 @@
         <v>30</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C6" s="18" t="s">
         <v>54</v>
@@ -2447,46 +2447,46 @@
         <v>15</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F6" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="G6" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="G6" s="20" t="s">
-        <v>167</v>
-      </c>
       <c r="H6" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="I6" s="18" t="s">
+      <c r="K6" s="20" t="s">
+        <v>173</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="N6" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="J6" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>174</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="M6" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="N6" s="18" t="s">
-        <v>150</v>
-      </c>
       <c r="O6" s="18" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="P6" s="18" t="s">
         <v>37</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="R6" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="S6" s="18" t="s">
         <v>37</v>
@@ -2508,7 +2508,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="18" t="s">
         <v>15</v>
@@ -2522,13 +2522,13 @@
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="18" t="s">
         <v>176</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>177</v>
       </c>
       <c r="D8" s="18" t="s">
         <v>15</v>
@@ -2542,13 +2542,13 @@
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" t="s">
         <v>15</v>
       </c>
       <c r="C9" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D9" s="18" t="s">
         <v>15</v>
@@ -2562,13 +2562,13 @@
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B10" t="s">
         <v>15</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D10" s="18" t="s">
         <v>15</v>
@@ -2582,13 +2582,13 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B11" t="s">
         <v>15</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D11" s="18" t="s">
         <v>15</v>
@@ -2602,13 +2602,13 @@
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>181</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>182</v>
       </c>
       <c r="D12" s="18" t="s">
         <v>15</v>
@@ -2622,13 +2622,13 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="18" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D13" s="18" t="s">
         <v>15</v>
@@ -2642,13 +2642,13 @@
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="18" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D14" s="18" t="s">
         <v>15</v>
@@ -2662,13 +2662,13 @@
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D15" s="18" t="s">
         <v>15</v>
@@ -2682,13 +2682,13 @@
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" s="18" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D16" s="18" t="s">
         <v>15</v>
@@ -2702,13 +2702,13 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A17" s="18" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
       </c>
       <c r="C17" s="18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D17" s="18" t="s">
         <v>15</v>
@@ -2722,55 +2722,55 @@
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A18" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="D18" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="18" t="s">
+      <c r="F18" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="H18" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="F18" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="G18" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="H18" s="18" t="s">
+      <c r="I18" s="18" t="s">
         <v>199</v>
       </c>
-      <c r="I18" s="18" t="s">
+      <c r="J18" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="K18" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="L18" s="18" t="s">
         <v>200</v>
       </c>
-      <c r="J18" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="K18" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="L18" s="18" t="s">
+      <c r="M18" s="22" t="s">
         <v>201</v>
       </c>
-      <c r="M18" s="22" t="s">
-        <v>202</v>
-      </c>
       <c r="N18" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O18" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P18" s="18" t="s">
         <v>37</v>
       </c>
       <c r="Q18" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="V18" s="18">
         <v>200</v>
@@ -2781,55 +2781,55 @@
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A19" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="B19" t="s">
         <v>205</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="C19" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="18" t="s">
+      <c r="F19" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="H19" s="18" t="s">
         <v>207</v>
       </c>
-      <c r="F19" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="H19" s="18" t="s">
+      <c r="I19" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K19" s="18" t="s">
+        <v>173</v>
+      </c>
+      <c r="L19" s="18" t="s">
         <v>208</v>
       </c>
-      <c r="I19" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K19" s="18" t="s">
-        <v>174</v>
-      </c>
-      <c r="L19" s="18" t="s">
+      <c r="M19" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="M19" s="22" t="s">
-        <v>210</v>
-      </c>
       <c r="N19" s="18" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O19" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P19" s="18" t="s">
         <v>37</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="V19" s="18">
         <v>404</v>
@@ -2840,49 +2840,49 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A20" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="B20" t="s">
         <v>211</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>212</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="D20" s="18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="18" t="s">
+      <c r="F20" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="K20" t="s">
+        <v>173</v>
+      </c>
+      <c r="L20" t="s">
         <v>213</v>
       </c>
-      <c r="F20" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="G20" s="18" t="s">
-        <v>167</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="K20" t="s">
-        <v>174</v>
-      </c>
-      <c r="L20" t="s">
-        <v>214</v>
-      </c>
       <c r="M20" s="24" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="P20" t="s">
         <v>37</v>
       </c>
       <c r="Q20" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="S20" t="s">
         <v>37</v>
@@ -2896,19 +2896,19 @@
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D21" s="18" t="s">
         <v>15</v>
       </c>
       <c r="R21" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S21" t="s">
         <v>37</v>
@@ -2922,19 +2922,19 @@
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="B22" t="s">
+        <v>221</v>
+      </c>
+      <c r="C22" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="B22" t="s">
-        <v>222</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>218</v>
-      </c>
       <c r="D22" s="18" t="s">
         <v>15</v>
       </c>
       <c r="R22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T22" t="s">
         <v>37</v>
@@ -2948,19 +2948,19 @@
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B23" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C23" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D23" s="18" t="s">
         <v>15</v>
       </c>
       <c r="R23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="T23" t="s">
         <v>37</v>
@@ -2974,13 +2974,13 @@
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A24" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="B24" t="s">
         <v>223</v>
       </c>
-      <c r="B24" t="s">
-        <v>224</v>
-      </c>
       <c r="C24" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D24" s="18" t="s">
         <v>15</v>
@@ -2997,13 +2997,13 @@
     </row>
     <row r="25" spans="1:23" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B25" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="V25" s="18">
         <v>200</v>
@@ -3014,13 +3014,13 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A26" s="18" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B26" t="s">
+        <v>227</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>228</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>229</v>
       </c>
       <c r="V26" s="18">
         <v>404</v>
@@ -3160,7 +3160,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B2" t="s">
         <v>59</v>
@@ -3181,7 +3181,7 @@
         <v>48</v>
       </c>
       <c r="I2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J2" t="s">
         <v>37</v>
@@ -3213,7 +3213,7 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" t="s">
         <v>57</v>
@@ -3254,7 +3254,7 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
         <v>58</v>
@@ -3292,7 +3292,7 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B5" t="s">
         <v>67</v>
@@ -3345,7 +3345,7 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
         <v>68</v>
@@ -3398,7 +3398,7 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>71</v>
@@ -3454,7 +3454,7 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B8" t="s">
         <v>72</v>
@@ -3480,7 +3480,7 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B9" t="s">
         <v>59</v>
@@ -3500,7 +3500,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>71</v>
@@ -3523,7 +3523,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B11" t="s">
         <v>74</v>
@@ -3543,7 +3543,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B12" t="s">
         <v>76</v>
@@ -3563,7 +3563,7 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B13" t="s">
         <v>78</v>
@@ -3586,7 +3586,7 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>71</v>
@@ -3609,7 +3609,7 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B15" t="s">
         <v>76</v>
@@ -3632,7 +3632,7 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B16" t="s">
         <v>80</v>
@@ -3655,7 +3655,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B17" t="s">
         <v>80</v>
@@ -3678,7 +3678,7 @@
     </row>
     <row r="18" spans="1:22" s="9" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A18" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>80</v>
@@ -3701,7 +3701,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>71</v>
@@ -3724,13 +3724,13 @@
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" t="s">
         <v>143</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>144</v>
-      </c>
-      <c r="C20" t="s">
-        <v>145</v>
       </c>
       <c r="D20" t="s">
         <v>15</v>

</xml_diff>